<commit_message>
add cloum remark for reg apple
</commit_message>
<xml_diff>
--- a/public/upload/files/reg_apple_example.xlsx
+++ b/public/upload/files/reg_apple_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\技术大牛初养成\make money\多用户邮件管理系统\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\phpstudy_pro\WWW\all-mail.im\public\upload\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A524D13-B0FC-46D2-8D98-7859348EE585}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F754CE-D8C5-44C2-957D-8FD1A4B21760}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="816" windowWidth="20364" windowHeight="11544" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>账号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -36,6 +36,14 @@
   </si>
   <si>
     <t>apple@163.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1组</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -380,7 +388,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -400,7 +408,9 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -413,7 +423,9 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>

</xml_diff>